<commit_message>
[assets][reports] minor corrections in assets
- remove backspace:
    - `Acquisition ID Image` (ORB-v1.0 item 2.5)
    - `Acquisition ID Image` (NRB-v5.5 item 2.8)
    - `Per-Pixel DEM` (NRB-v5.5 item 2.9)
    - `Backscatter Conversion` (NRB-v5.0 & NRB-v5.5 item 3.2)
- remove additional space:
    - `Radiometric Accuracy` (ORB-v1.0 item 3.3)
</commit_message>
<xml_diff>
--- a/assets/nrb/CARD4L_METADATA-spec_NRB-v5.0.xlsx
+++ b/assets/nrb/CARD4L_METADATA-spec_NRB-v5.0.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcowo/Documents/pypypy/ceos-ard-spec-tables/assets/nrb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3459D5-F66C-8B43-8D46-2711D0611AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4D1A52-E837-4F4B-83BB-B41FE63BCF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="760" windowWidth="33480" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="760" windowWidth="33480" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1st page" sheetId="5" r:id="rId1"/>
@@ -811,32 +811,6 @@
   </si>
   <si>
     <t>Backscatter Measurements</t>
-  </si>
-  <si>
-    <r>
-      <t>Backscatter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                          </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Conversion </t>
-    </r>
   </si>
   <si>
     <t>&lt;BackscatterMeasurementData&gt;</t>
@@ -1280,6 +1254,9 @@
   </si>
   <si>
     <t>&lt;SourceDataAcquisitionTime&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backscatter Conversion </t>
   </si>
 </sst>
 </file>
@@ -2545,6 +2522,90 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="16" fillId="3" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2557,18 +2618,6 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2578,129 +2627,57 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2710,74 +2687,74 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3174,269 +3151,269 @@
       <c r="B2" s="78"/>
       <c r="C2" s="53"/>
       <c r="D2" s="79"/>
-      <c r="E2" s="120" t="s">
-        <v>220</v>
-      </c>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="129" t="s">
-        <v>231</v>
-      </c>
-      <c r="I2" s="130"/>
-      <c r="J2" s="131"/>
+      <c r="E2" s="109" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="110"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="118" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="119"/>
+      <c r="J2" s="120"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="80"/>
       <c r="D3" s="81"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="134"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="80"/>
       <c r="D4" s="81"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="134"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="123"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="80"/>
       <c r="D5" s="81"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="134"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="123"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="80"/>
       <c r="D6" s="81"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="134"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="123"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="80"/>
       <c r="D7" s="81"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="134"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="123"/>
     </row>
     <row r="8" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="82"/>
       <c r="C8" s="83"/>
       <c r="D8" s="84"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="137"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="126"/>
     </row>
     <row r="12" spans="2:10" s="85" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B12" s="85" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:10" s="51" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="88" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="127" t="s">
         <v>222</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="D14" s="127"/>
+      <c r="E14" s="127" t="s">
         <v>223</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138" t="s">
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127" t="s">
         <v>224</v>
       </c>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138" t="s">
-        <v>225</v>
-      </c>
-      <c r="J14" s="139"/>
+      <c r="J14" s="128"/>
     </row>
     <row r="15" spans="2:10" s="51" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="87">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C15" s="116" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="117"/>
-      <c r="E15" s="118" t="s">
+      <c r="C15" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="106"/>
+      <c r="E15" s="107" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118" t="s">
-        <v>227</v>
-      </c>
-      <c r="J15" s="119"/>
+      <c r="J15" s="108"/>
     </row>
     <row r="16" spans="2:10" s="51" customFormat="1" ht="76.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="86">
         <v>4.2</v>
       </c>
-      <c r="C16" s="109" t="s">
-        <v>238</v>
-      </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="111" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111" t="s">
+      <c r="C16" s="129" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="130"/>
+      <c r="E16" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="J16" s="112"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="131" t="s">
+        <v>227</v>
+      </c>
+      <c r="J16" s="132"/>
     </row>
     <row r="17" spans="2:10" s="51" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="86">
         <v>4.5</v>
       </c>
-      <c r="C17" s="109" t="s">
-        <v>239</v>
-      </c>
-      <c r="D17" s="110"/>
-      <c r="E17" s="111" t="s">
-        <v>232</v>
-      </c>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111" t="s">
-        <v>322</v>
-      </c>
-      <c r="J17" s="112"/>
+      <c r="C17" s="129" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="130"/>
+      <c r="E17" s="131" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131" t="s">
+        <v>321</v>
+      </c>
+      <c r="J17" s="132"/>
     </row>
     <row r="18" spans="2:10" s="51" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B18" s="86">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C18" s="109" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="111" t="s">
-        <v>230</v>
-      </c>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111" t="s">
-        <v>228</v>
-      </c>
-      <c r="J18" s="112"/>
+      <c r="C18" s="129" t="s">
+        <v>239</v>
+      </c>
+      <c r="D18" s="130"/>
+      <c r="E18" s="131" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18" s="131"/>
+      <c r="G18" s="131"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="131" t="s">
+        <v>227</v>
+      </c>
+      <c r="J18" s="132"/>
     </row>
     <row r="19" spans="2:10" s="51" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B19" s="86">
         <v>4.7</v>
       </c>
-      <c r="C19" s="109" t="s">
-        <v>236</v>
-      </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="111" t="s">
-        <v>234</v>
-      </c>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111" t="s">
-        <v>227</v>
-      </c>
-      <c r="J19" s="112"/>
+      <c r="C19" s="129" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="130"/>
+      <c r="E19" s="131" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="131"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="131" t="s">
+        <v>226</v>
+      </c>
+      <c r="J19" s="132"/>
     </row>
     <row r="20" spans="2:10" s="51" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B20" s="86">
         <v>4.8</v>
       </c>
-      <c r="C20" s="109" t="s">
-        <v>235</v>
-      </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="111" t="s">
-        <v>241</v>
-      </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111" t="s">
-        <v>227</v>
-      </c>
-      <c r="J20" s="112"/>
+      <c r="C20" s="129" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" s="130"/>
+      <c r="E20" s="131" t="s">
+        <v>240</v>
+      </c>
+      <c r="F20" s="131"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="131"/>
+      <c r="I20" s="131" t="s">
+        <v>226</v>
+      </c>
+      <c r="J20" s="132"/>
     </row>
     <row r="21" spans="2:10" s="51" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="86">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="129" t="s">
+        <v>241</v>
+      </c>
+      <c r="D21" s="130"/>
+      <c r="E21" s="137" t="s">
         <v>242</v>
       </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="113" t="s">
-        <v>243</v>
-      </c>
-      <c r="F21" s="114"/>
-      <c r="G21" s="114"/>
-      <c r="H21" s="115"/>
-      <c r="I21" s="111" t="s">
-        <v>228</v>
-      </c>
-      <c r="J21" s="112"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="131" t="s">
+        <v>227</v>
+      </c>
+      <c r="J21" s="132"/>
     </row>
     <row r="22" spans="2:10" s="51" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="103" t="s">
-        <v>326</v>
-      </c>
-      <c r="C22" s="105" t="s">
-        <v>242</v>
-      </c>
-      <c r="D22" s="106"/>
-      <c r="E22" s="107" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="133" t="s">
+        <v>241</v>
+      </c>
+      <c r="D22" s="134"/>
+      <c r="E22" s="135" t="s">
+        <v>243</v>
+      </c>
+      <c r="F22" s="135"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="135" t="s">
         <v>244</v>
       </c>
-      <c r="F22" s="107"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="107"/>
-      <c r="I22" s="107" t="s">
-        <v>245</v>
-      </c>
-      <c r="J22" s="108"/>
+      <c r="J22" s="136"/>
     </row>
     <row r="23" spans="2:10" s="101" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:10" s="101" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B24" s="102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="2:10" s="101" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B25" s="102" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="2:10" s="101" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B26" s="102" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27" spans="2:10" s="101" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
@@ -3444,26 +3421,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="29">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="E2:G8"/>
-    <mergeCell ref="H2:J8"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="I22:J22"/>
@@ -3473,6 +3430,26 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="E2:G8"/>
+    <mergeCell ref="H2:J8"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="I14:J14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3492,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BI231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -3509,30 +3486,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="104" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="140" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
+      <c r="A2" s="155" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
     </row>
     <row r="3" spans="1:6" s="104" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="E4" s="143" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -3540,64 +3517,64 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="154"/>
-      <c r="B5" s="156"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
+      <c r="A5" s="144"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="141">
+      <c r="A6" s="140">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="140" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="89"/>
       <c r="E6" s="90"/>
       <c r="F6" s="91"/>
     </row>
     <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="143"/>
-      <c r="B7" s="143"/>
+      <c r="A7" s="142"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="148"/>
       <c r="D7" s="92"/>
       <c r="E7" s="93"/>
       <c r="F7" s="94"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="141">
+      <c r="A8" s="140">
         <v>1.2</v>
       </c>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="145" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="147" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="89"/>
       <c r="E8" s="90"/>
       <c r="F8" s="91"/>
     </row>
     <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="142"/>
-      <c r="B9" s="145"/>
+      <c r="A9" s="141"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="148"/>
       <c r="D9" s="92"/>
       <c r="E9" s="93"/>
       <c r="F9" s="94"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="141">
+      <c r="A10" s="140">
         <v>1.3</v>
       </c>
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="140" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3"/>
@@ -3606,32 +3583,32 @@
       <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="142"/>
-      <c r="B11" s="142"/>
+      <c r="A11" s="141"/>
+      <c r="B11" s="141"/>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
-      <c r="B12" s="143"/>
+      <c r="A12" s="142"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="4"/>
       <c r="D12" s="14"/>
       <c r="E12" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="141">
+      <c r="A13" s="140">
         <v>1.4</v>
       </c>
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="140" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3"/>
@@ -3640,22 +3617,22 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="143"/>
+      <c r="A14" s="142"/>
+      <c r="B14" s="142"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
       <c r="F14" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="141">
+      <c r="A15" s="140">
         <v>1.5</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="140" t="s">
         <v>191</v>
       </c>
       <c r="C15" s="3"/>
@@ -3664,8 +3641,8 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="142"/>
-      <c r="B16" s="142"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="3" t="s">
         <v>192</v>
       </c>
@@ -3674,46 +3651,46 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="142"/>
-      <c r="B17" s="142"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="142"/>
-      <c r="B18" s="142"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
-      <c r="B19" s="143"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="141">
+      <c r="A20" s="140">
         <v>1.6</v>
       </c>
-      <c r="B20" s="141" t="s">
+      <c r="B20" s="140" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
@@ -3722,24 +3699,24 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="142"/>
-      <c r="B21" s="142"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="141"/>
       <c r="C21" s="36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="141" t="s">
+      <c r="A22" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="140" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -3752,32 +3729,32 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="142"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="141"/>
       <c r="C23" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
-      <c r="B24" s="143"/>
+      <c r="A24" s="142"/>
+      <c r="B24" s="142"/>
       <c r="C24" s="8"/>
       <c r="D24" s="14"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="141" t="s">
+      <c r="A25" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="140" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3"/>
@@ -3786,34 +3763,34 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="142"/>
-      <c r="B26" s="142"/>
+      <c r="A26" s="141"/>
+      <c r="B26" s="141"/>
       <c r="C26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="16"/>
       <c r="F26" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="142"/>
-      <c r="B27" s="142"/>
+      <c r="A27" s="141"/>
+      <c r="B27" s="141"/>
       <c r="C27" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D27" s="46"/>
       <c r="E27" s="35"/>
       <c r="F27" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="141" t="s">
+      <c r="A28" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="145" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="39"/>
@@ -3822,42 +3799,42 @@
       <c r="F28" s="32"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="142"/>
-      <c r="B29" s="145"/>
+      <c r="A29" s="141"/>
+      <c r="B29" s="146"/>
       <c r="C29" s="40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="16"/>
       <c r="F29" s="41"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="142"/>
-      <c r="B30" s="145"/>
+      <c r="A30" s="141"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="40" t="s">
         <v>188</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="16"/>
       <c r="F30" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="142"/>
-      <c r="B31" s="145"/>
+      <c r="A31" s="141"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="40" t="s">
         <v>133</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="16"/>
       <c r="F31" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="143"/>
-      <c r="B32" s="146"/>
+      <c r="A32" s="142"/>
+      <c r="B32" s="156"/>
       <c r="C32" s="42"/>
       <c r="D32" s="36"/>
       <c r="E32" s="35"/>
@@ -3866,10 +3843,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="141" t="s">
+      <c r="A33" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="141" t="s">
+      <c r="B33" s="140" t="s">
         <v>206</v>
       </c>
       <c r="C33" s="10"/>
@@ -3878,8 +3855,8 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="142"/>
-      <c r="B34" s="142"/>
+      <c r="A34" s="141"/>
+      <c r="B34" s="141"/>
       <c r="C34" s="3" t="s">
         <v>21</v>
       </c>
@@ -3888,84 +3865,84 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="142"/>
-      <c r="B35" s="142"/>
+      <c r="A35" s="141"/>
+      <c r="B35" s="141"/>
       <c r="C35" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="142"/>
-      <c r="B36" s="142"/>
+      <c r="A36" s="141"/>
+      <c r="B36" s="141"/>
       <c r="C36" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="142"/>
-      <c r="B37" s="142"/>
+      <c r="A37" s="141"/>
+      <c r="B37" s="141"/>
       <c r="C37" s="3" t="s">
         <v>136</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="10"/>
       <c r="F37" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="142"/>
-      <c r="B38" s="142"/>
+      <c r="A38" s="141"/>
+      <c r="B38" s="141"/>
       <c r="C38" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="10"/>
       <c r="F38" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="142"/>
-      <c r="B39" s="142"/>
+      <c r="A39" s="141"/>
+      <c r="B39" s="141"/>
       <c r="C39" s="3" t="s">
         <v>189</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="10"/>
       <c r="F39" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="143"/>
-      <c r="B40" s="143"/>
+      <c r="A40" s="142"/>
+      <c r="B40" s="142"/>
       <c r="C40" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="8"/>
       <c r="F40" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="141" t="s">
+      <c r="A41" s="140" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="141" t="s">
+      <c r="B41" s="140" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="3"/>
@@ -3974,8 +3951,8 @@
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="142"/>
-      <c r="B42" s="142"/>
+      <c r="A42" s="141"/>
+      <c r="B42" s="141"/>
       <c r="C42" s="3" t="s">
         <v>23</v>
       </c>
@@ -3984,74 +3961,74 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="142"/>
-      <c r="B43" s="142"/>
+      <c r="A43" s="141"/>
+      <c r="B43" s="141"/>
       <c r="C43" s="3" t="s">
         <v>139</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="142"/>
-      <c r="B44" s="142"/>
+      <c r="A44" s="141"/>
+      <c r="B44" s="141"/>
       <c r="C44" s="3" t="s">
         <v>140</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="5"/>
       <c r="F44" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="142"/>
-      <c r="B45" s="142"/>
+      <c r="A45" s="141"/>
+      <c r="B45" s="141"/>
       <c r="C45" s="5"/>
       <c r="D45" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="142"/>
-      <c r="B46" s="142"/>
+      <c r="A46" s="141"/>
+      <c r="B46" s="141"/>
       <c r="C46" s="10"/>
       <c r="D46" s="3" t="s">
         <v>143</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="143"/>
-      <c r="B47" s="143"/>
+      <c r="A47" s="142"/>
+      <c r="B47" s="142"/>
       <c r="C47" s="8"/>
       <c r="D47" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="141" t="s">
+      <c r="A48" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="141" t="s">
+      <c r="B48" s="140" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="98"/>
@@ -4060,8 +4037,8 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="142"/>
-      <c r="B49" s="142"/>
+      <c r="A49" s="141"/>
+      <c r="B49" s="141"/>
       <c r="C49" s="63" t="s">
         <v>25</v>
       </c>
@@ -4072,138 +4049,138 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="142"/>
-      <c r="B50" s="142"/>
+      <c r="A50" s="141"/>
+      <c r="B50" s="141"/>
       <c r="C50" s="63" t="s">
         <v>144</v>
       </c>
       <c r="D50" s="59"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="142"/>
-      <c r="B51" s="142"/>
+      <c r="A51" s="141"/>
+      <c r="B51" s="141"/>
       <c r="C51" s="63" t="s">
         <v>145</v>
       </c>
       <c r="D51" s="59"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="142"/>
-      <c r="B52" s="142"/>
+      <c r="A52" s="141"/>
+      <c r="B52" s="141"/>
       <c r="C52" s="63" t="s">
         <v>146</v>
       </c>
       <c r="D52" s="70"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="142"/>
-      <c r="B53" s="142"/>
+      <c r="A53" s="141"/>
+      <c r="B53" s="141"/>
       <c r="C53" s="63" t="s">
         <v>147</v>
       </c>
       <c r="D53" s="70"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="142"/>
-      <c r="B54" s="142"/>
+      <c r="A54" s="141"/>
+      <c r="B54" s="141"/>
       <c r="C54" s="63" t="s">
         <v>148</v>
       </c>
       <c r="D54" s="70"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="142"/>
-      <c r="B55" s="142"/>
+      <c r="A55" s="141"/>
+      <c r="B55" s="141"/>
       <c r="C55" s="63" t="s">
         <v>150</v>
       </c>
       <c r="D55" s="59"/>
       <c r="E55" s="95" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="142"/>
-      <c r="B56" s="142"/>
+      <c r="A56" s="141"/>
+      <c r="B56" s="141"/>
       <c r="C56" s="63"/>
       <c r="D56" s="59" t="s">
         <v>151</v>
       </c>
       <c r="E56" s="95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="142"/>
-      <c r="B57" s="142"/>
+      <c r="A57" s="141"/>
+      <c r="B57" s="141"/>
       <c r="C57" s="63" t="s">
         <v>149</v>
       </c>
       <c r="D57" s="100"/>
       <c r="E57" s="95" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="142"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="141"/>
+      <c r="B58" s="141"/>
       <c r="C58" s="63"/>
       <c r="D58" s="59" t="s">
         <v>152</v>
       </c>
       <c r="E58" s="95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="141"/>
+      <c r="B59" s="141"/>
       <c r="C59" s="99"/>
       <c r="D59" s="62" t="s">
         <v>190</v>
       </c>
       <c r="E59" s="43"/>
       <c r="F59" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="141" t="s">
+      <c r="A60" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="141" t="s">
+      <c r="B60" s="140" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="5"/>
@@ -4212,8 +4189,8 @@
       <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="142"/>
-      <c r="B61" s="142"/>
+      <c r="A61" s="141"/>
+      <c r="B61" s="141"/>
       <c r="C61" s="3" t="s">
         <v>27</v>
       </c>
@@ -4224,8 +4201,8 @@
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="142"/>
-      <c r="B62" s="142"/>
+      <c r="A62" s="141"/>
+      <c r="B62" s="141"/>
       <c r="C62" s="3" t="s">
         <v>153</v>
       </c>
@@ -4233,85 +4210,85 @@
         <v>17</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="142"/>
-      <c r="B63" s="142"/>
+      <c r="A63" s="141"/>
+      <c r="B63" s="141"/>
       <c r="C63" s="3" t="s">
         <v>154</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="142"/>
-      <c r="B64" s="142"/>
+      <c r="A64" s="141"/>
+      <c r="B64" s="141"/>
       <c r="C64" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="142"/>
-      <c r="B65" s="142"/>
+      <c r="A65" s="141"/>
+      <c r="B65" s="141"/>
       <c r="C65" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="142"/>
-      <c r="B66" s="142"/>
+      <c r="A66" s="141"/>
+      <c r="B66" s="141"/>
       <c r="C66" s="23" t="s">
         <v>157</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="142"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="141"/>
+      <c r="B67" s="141"/>
       <c r="C67" s="3" t="s">
         <v>158</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="142"/>
-      <c r="B68" s="142"/>
+      <c r="A68" s="141"/>
+      <c r="B68" s="141"/>
       <c r="C68" s="3" t="s">
         <v>16</v>
       </c>
@@ -4319,57 +4296,57 @@
         <v>159</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="142"/>
-      <c r="B69" s="142"/>
+      <c r="A69" s="141"/>
+      <c r="B69" s="141"/>
       <c r="C69" s="10"/>
       <c r="D69" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="142"/>
-      <c r="B70" s="142"/>
+      <c r="A70" s="141"/>
+      <c r="B70" s="141"/>
       <c r="C70" s="10"/>
       <c r="D70" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="143"/>
-      <c r="B71" s="143"/>
+      <c r="A71" s="142"/>
+      <c r="B71" s="142"/>
       <c r="C71" s="10"/>
       <c r="D71" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="141" t="s">
+      <c r="A72" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="144" t="s">
+      <c r="B72" s="145" t="s">
         <v>30</v>
       </c>
       <c r="C72" s="39"/>
@@ -4378,24 +4355,24 @@
       <c r="F72" s="32"/>
     </row>
     <row r="73" spans="1:6" s="49" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="142"/>
-      <c r="B73" s="145"/>
+      <c r="A73" s="141"/>
+      <c r="B73" s="146"/>
       <c r="C73" s="97"/>
       <c r="D73" s="36" t="s">
         <v>31</v>
       </c>
       <c r="E73" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F73" s="34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="141" t="s">
+      <c r="A74" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="B74" s="141" t="s">
+      <c r="B74" s="140" t="s">
         <v>32</v>
       </c>
       <c r="C74" s="3"/>
@@ -4408,34 +4385,34 @@
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="142"/>
-      <c r="B75" s="142"/>
+      <c r="A75" s="141"/>
+      <c r="B75" s="141"/>
       <c r="C75" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="142"/>
-      <c r="B76" s="142"/>
+      <c r="A76" s="141"/>
+      <c r="B76" s="141"/>
       <c r="C76" s="3" t="s">
         <v>160</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="142"/>
-      <c r="B77" s="142"/>
+      <c r="A77" s="141"/>
+      <c r="B77" s="141"/>
       <c r="C77" s="3" t="s">
         <v>34</v>
       </c>
@@ -4443,55 +4420,55 @@
         <v>161</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="142"/>
-      <c r="B78" s="142"/>
+      <c r="A78" s="141"/>
+      <c r="B78" s="141"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
         <v>162</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="142"/>
-      <c r="B79" s="142"/>
+      <c r="A79" s="141"/>
+      <c r="B79" s="141"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
         <v>163</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="142"/>
-      <c r="B80" s="142"/>
+      <c r="A80" s="141"/>
+      <c r="B80" s="141"/>
       <c r="C80" s="3"/>
       <c r="D80" s="36" t="s">
         <v>164</v>
       </c>
       <c r="E80" s="44"/>
       <c r="F80" s="44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="141" t="s">
+      <c r="A81" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="B81" s="141" t="s">
+      <c r="B81" s="140" t="s">
         <v>35</v>
       </c>
       <c r="C81" s="21"/>
@@ -4502,22 +4479,22 @@
       <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6" ht="22.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="142"/>
-      <c r="B82" s="142"/>
+      <c r="A82" s="141"/>
+      <c r="B82" s="141"/>
       <c r="C82" s="14"/>
       <c r="D82" s="36" t="s">
         <v>36</v>
       </c>
       <c r="E82" s="44"/>
       <c r="F82" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="141" t="s">
+      <c r="A83" s="140" t="s">
         <v>194</v>
       </c>
-      <c r="B83" s="141" t="s">
+      <c r="B83" s="140" t="s">
         <v>37</v>
       </c>
       <c r="C83" s="21"/>
@@ -4528,38 +4505,38 @@
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="142"/>
-      <c r="B84" s="142"/>
+      <c r="A84" s="141"/>
+      <c r="B84" s="141"/>
       <c r="C84" s="22"/>
       <c r="D84" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="143"/>
-      <c r="B85" s="143"/>
+      <c r="A85" s="142"/>
+      <c r="B85" s="142"/>
       <c r="C85" s="14"/>
       <c r="D85" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="141" t="s">
+      <c r="A86" s="140" t="s">
         <v>195</v>
       </c>
-      <c r="B86" s="141" t="s">
+      <c r="B86" s="140" t="s">
         <v>40</v>
       </c>
       <c r="C86" s="20"/>
@@ -4570,22 +4547,22 @@
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="142"/>
-      <c r="B87" s="142"/>
+      <c r="A87" s="141"/>
+      <c r="B87" s="141"/>
       <c r="C87" s="35"/>
       <c r="D87" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E87" s="35"/>
       <c r="F87" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="141">
+      <c r="A88" s="140">
         <v>1.7</v>
       </c>
-      <c r="B88" s="141" t="s">
+      <c r="B88" s="140" t="s">
         <v>42</v>
       </c>
       <c r="C88" s="3"/>
@@ -4596,22 +4573,22 @@
       <c r="F88" s="32"/>
     </row>
     <row r="89" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="142"/>
-      <c r="B89" s="142"/>
+      <c r="A89" s="141"/>
+      <c r="B89" s="141"/>
       <c r="C89" s="36" t="s">
         <v>43</v>
       </c>
       <c r="D89" s="48"/>
       <c r="E89" s="38"/>
       <c r="F89" s="34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="141" t="s">
+      <c r="A90" s="140" t="s">
         <v>196</v>
       </c>
-      <c r="B90" s="141" t="s">
+      <c r="B90" s="140" t="s">
         <v>45</v>
       </c>
       <c r="C90" s="3"/>
@@ -4622,8 +4599,8 @@
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="142"/>
-      <c r="B91" s="142"/>
+      <c r="A91" s="141"/>
+      <c r="B91" s="141"/>
       <c r="C91" s="3" t="s">
         <v>46</v>
       </c>
@@ -4632,60 +4609,60 @@
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="142"/>
-      <c r="B92" s="142"/>
+      <c r="A92" s="141"/>
+      <c r="B92" s="141"/>
       <c r="C92" s="3" t="s">
         <v>144</v>
       </c>
       <c r="D92" s="22"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="142"/>
-      <c r="B93" s="142"/>
+      <c r="A93" s="141"/>
+      <c r="B93" s="141"/>
       <c r="C93" s="3" t="s">
         <v>165</v>
       </c>
       <c r="D93" s="22"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="142"/>
-      <c r="B94" s="142"/>
+      <c r="A94" s="141"/>
+      <c r="B94" s="141"/>
       <c r="C94" s="3" t="s">
         <v>146</v>
       </c>
       <c r="D94" s="22"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="143"/>
-      <c r="B95" s="143"/>
+      <c r="A95" s="142"/>
+      <c r="B95" s="142"/>
       <c r="C95" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D95" s="14"/>
       <c r="E95" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="141" t="s">
+      <c r="A96" s="140" t="s">
         <v>197</v>
       </c>
-      <c r="B96" s="141" t="s">
+      <c r="B96" s="140" t="s">
         <v>48</v>
       </c>
       <c r="C96" s="12"/>
@@ -4694,24 +4671,24 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="143"/>
-      <c r="B97" s="143"/>
+      <c r="A97" s="142"/>
+      <c r="B97" s="142"/>
       <c r="C97" s="13" t="s">
         <v>49</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="141" t="s">
+      <c r="A98" s="140" t="s">
         <v>198</v>
       </c>
-      <c r="B98" s="141" t="s">
+      <c r="B98" s="140" t="s">
         <v>51</v>
       </c>
       <c r="C98" s="5"/>
@@ -4722,8 +4699,8 @@
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="142"/>
-      <c r="B99" s="142"/>
+      <c r="A99" s="141"/>
+      <c r="B99" s="141"/>
       <c r="C99" s="3" t="s">
         <v>52</v>
       </c>
@@ -4732,34 +4709,34 @@
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="142"/>
-      <c r="B100" s="142"/>
+      <c r="A100" s="141"/>
+      <c r="B100" s="141"/>
       <c r="C100" s="3" t="s">
         <v>167</v>
       </c>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
       <c r="F100" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="142"/>
-      <c r="B101" s="142"/>
+      <c r="A101" s="141"/>
+      <c r="B101" s="141"/>
       <c r="C101" s="36" t="s">
         <v>168</v>
       </c>
       <c r="D101" s="35"/>
       <c r="E101" s="35"/>
       <c r="F101" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="141" t="s">
+      <c r="A102" s="140" t="s">
         <v>199</v>
       </c>
-      <c r="B102" s="141" t="s">
+      <c r="B102" s="140" t="s">
         <v>54</v>
       </c>
       <c r="C102" s="5"/>
@@ -4770,8 +4747,8 @@
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="142"/>
-      <c r="B103" s="142"/>
+      <c r="A103" s="141"/>
+      <c r="B103" s="141"/>
       <c r="C103" s="3" t="s">
         <v>55</v>
       </c>
@@ -4780,56 +4757,56 @@
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="142"/>
-      <c r="B104" s="142"/>
+      <c r="A104" s="141"/>
+      <c r="B104" s="141"/>
       <c r="C104" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D104" s="16"/>
       <c r="E104" s="16"/>
       <c r="F104" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="142"/>
-      <c r="B105" s="142"/>
+      <c r="A105" s="141"/>
+      <c r="B105" s="141"/>
       <c r="C105" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D105" s="16"/>
       <c r="E105" s="16"/>
       <c r="F105" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="142"/>
-      <c r="B106" s="142"/>
+      <c r="A106" s="141"/>
+      <c r="B106" s="141"/>
       <c r="C106" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D106" s="16"/>
       <c r="E106" s="16"/>
       <c r="F106" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="142"/>
-      <c r="B107" s="142"/>
+      <c r="A107" s="141"/>
+      <c r="B107" s="141"/>
       <c r="C107" s="3" t="s">
         <v>170</v>
       </c>
       <c r="D107" s="16"/>
       <c r="E107" s="16"/>
       <c r="F107" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="143"/>
-      <c r="B108" s="143"/>
+      <c r="A108" s="142"/>
+      <c r="B108" s="142"/>
       <c r="C108" s="4" t="s">
         <v>57</v>
       </c>
@@ -4838,10 +4815,10 @@
       <c r="F108" s="8"/>
     </row>
     <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="141" t="s">
+      <c r="A109" s="140" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="141" t="s">
+      <c r="B109" s="140" t="s">
         <v>59</v>
       </c>
       <c r="C109" s="5"/>
@@ -4852,64 +4829,64 @@
       <c r="F109" s="5"/>
     </row>
     <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="142"/>
-      <c r="B110" s="142"/>
+      <c r="A110" s="141"/>
+      <c r="B110" s="141"/>
       <c r="C110" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F110" s="5"/>
     </row>
     <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="142"/>
-      <c r="B111" s="142"/>
+      <c r="A111" s="141"/>
+      <c r="B111" s="141"/>
       <c r="C111" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D111" s="16"/>
       <c r="E111" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="142"/>
-      <c r="B112" s="142"/>
+      <c r="A112" s="141"/>
+      <c r="B112" s="141"/>
       <c r="C112" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="143"/>
-      <c r="B113" s="143"/>
+      <c r="A113" s="142"/>
+      <c r="B113" s="142"/>
       <c r="C113" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D113" s="15"/>
       <c r="E113" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="141" t="s">
+      <c r="A114" s="140" t="s">
         <v>201</v>
       </c>
-      <c r="B114" s="141" t="s">
+      <c r="B114" s="140" t="s">
         <v>63</v>
       </c>
       <c r="C114" s="5"/>
@@ -4920,64 +4897,64 @@
       <c r="F114" s="5"/>
     </row>
     <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="142"/>
-      <c r="B115" s="142"/>
+      <c r="A115" s="141"/>
+      <c r="B115" s="141"/>
       <c r="C115" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F115" s="5"/>
     </row>
     <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="142"/>
-      <c r="B116" s="142"/>
+      <c r="A116" s="141"/>
+      <c r="B116" s="141"/>
       <c r="C116" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D116" s="16"/>
       <c r="E116" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="142"/>
-      <c r="B117" s="142"/>
+      <c r="A117" s="141"/>
+      <c r="B117" s="141"/>
       <c r="C117" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D117" s="16"/>
       <c r="E117" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="143"/>
-      <c r="B118" s="143"/>
+      <c r="A118" s="142"/>
+      <c r="B118" s="142"/>
       <c r="C118" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D118" s="15"/>
       <c r="E118" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="141" t="s">
+      <c r="A119" s="140" t="s">
         <v>202</v>
       </c>
-      <c r="B119" s="141" t="s">
+      <c r="B119" s="140" t="s">
         <v>66</v>
       </c>
       <c r="C119" s="5"/>
@@ -4986,8 +4963,8 @@
       <c r="F119" s="5"/>
     </row>
     <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="142"/>
-      <c r="B120" s="142"/>
+      <c r="A120" s="141"/>
+      <c r="B120" s="141"/>
       <c r="C120" s="3" t="s">
         <v>67</v>
       </c>
@@ -4996,60 +4973,60 @@
       <c r="F120" s="5"/>
     </row>
     <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="142"/>
-      <c r="B121" s="142"/>
+      <c r="A121" s="141"/>
+      <c r="B121" s="141"/>
       <c r="C121" s="3" t="s">
         <v>171</v>
       </c>
       <c r="D121" s="16"/>
       <c r="E121" s="5"/>
       <c r="F121" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="142"/>
-      <c r="B122" s="142"/>
+      <c r="A122" s="141"/>
+      <c r="B122" s="141"/>
       <c r="C122" s="3" t="s">
         <v>172</v>
       </c>
       <c r="D122" s="16"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="142"/>
-      <c r="B123" s="142"/>
+      <c r="A123" s="141"/>
+      <c r="B123" s="141"/>
       <c r="C123" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D123" s="16"/>
       <c r="E123" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="142"/>
-      <c r="B124" s="142"/>
+      <c r="A124" s="141"/>
+      <c r="B124" s="141"/>
       <c r="C124" s="22" t="s">
         <v>174</v>
       </c>
       <c r="D124" s="35"/>
       <c r="E124" s="28"/>
       <c r="F124" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="149" t="s">
+      <c r="A125" s="151" t="s">
         <v>203</v>
       </c>
-      <c r="B125" s="151" t="s">
+      <c r="B125" s="153" t="s">
         <v>69</v>
       </c>
       <c r="C125" s="29"/>
@@ -5060,22 +5037,22 @@
       <c r="F125" s="32"/>
     </row>
     <row r="126" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="150"/>
-      <c r="B126" s="152"/>
+      <c r="A126" s="152"/>
+      <c r="B126" s="154"/>
       <c r="C126" s="33" t="s">
         <v>70</v>
       </c>
       <c r="D126" s="36"/>
       <c r="E126" s="35"/>
       <c r="F126" s="34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="142" t="s">
+      <c r="A127" s="141" t="s">
         <v>204</v>
       </c>
-      <c r="B127" s="142" t="s">
+      <c r="B127" s="141" t="s">
         <v>72</v>
       </c>
       <c r="C127" s="3"/>
@@ -5086,22 +5063,22 @@
       <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="143"/>
-      <c r="B128" s="143"/>
+      <c r="A128" s="142"/>
+      <c r="B128" s="142"/>
       <c r="C128" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D128" s="14"/>
       <c r="E128" s="15"/>
       <c r="F128" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="141" t="s">
+      <c r="A129" s="140" t="s">
         <v>205</v>
       </c>
-      <c r="B129" s="141" t="s">
+      <c r="B129" s="140" t="s">
         <v>75</v>
       </c>
       <c r="C129" s="5"/>
@@ -5112,32 +5089,32 @@
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A130" s="142"/>
-      <c r="B130" s="142"/>
+      <c r="A130" s="141"/>
+      <c r="B130" s="141"/>
       <c r="C130" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D130" s="16"/>
       <c r="E130" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A131" s="142"/>
-      <c r="B131" s="142"/>
+      <c r="A131" s="141"/>
+      <c r="B131" s="141"/>
       <c r="C131" s="3" t="s">
         <v>175</v>
       </c>
       <c r="D131" s="16"/>
       <c r="E131" s="5"/>
       <c r="F131" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="143"/>
-      <c r="B132" s="143"/>
+      <c r="A132" s="142"/>
+      <c r="B132" s="142"/>
       <c r="C132" s="4" t="s">
         <v>77</v>
       </c>
@@ -5256,6 +5233,56 @@
     <row r="231" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A48:A59"/>
+    <mergeCell ref="B48:B59"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="A102:A108"/>
+    <mergeCell ref="B102:B108"/>
+    <mergeCell ref="B60:B71"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="A90:A95"/>
+    <mergeCell ref="B90:B95"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A129:A132"/>
+    <mergeCell ref="B129:B132"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="A119:A124"/>
+    <mergeCell ref="B119:B124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="A74:A80"/>
+    <mergeCell ref="B74:B80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
     <mergeCell ref="A60:A71"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
@@ -5272,56 +5299,6 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A74:A80"/>
-    <mergeCell ref="B74:B80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="A129:A132"/>
-    <mergeCell ref="B129:B132"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="A119:A124"/>
-    <mergeCell ref="B119:B124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="A48:A59"/>
-    <mergeCell ref="B48:B59"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="B127:B128"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="A102:A108"/>
-    <mergeCell ref="B102:B108"/>
-    <mergeCell ref="B60:B71"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="A90:A95"/>
-    <mergeCell ref="B90:B95"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="4" orientation="portrait"/>
@@ -5352,30 +5329,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="104" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="155" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
     </row>
     <row r="3" spans="1:6" s="104" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="E4" s="143" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -5383,11 +5360,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="154"/>
-      <c r="B5" s="156"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
+      <c r="A5" s="144"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
@@ -5396,11 +5373,11 @@
       <c r="A6" s="157">
         <v>2.1</v>
       </c>
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="140" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="89"/>
       <c r="E6" s="90"/>
@@ -5408,7 +5385,7 @@
     </row>
     <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="159"/>
-      <c r="B7" s="143"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="148"/>
       <c r="D7" s="92"/>
       <c r="E7" s="93"/>
@@ -5418,7 +5395,7 @@
       <c r="A8" s="157">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="140" t="s">
         <v>80</v>
       </c>
       <c r="C8" s="3"/>
@@ -5428,7 +5405,7 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="158"/>
-      <c r="B9" s="142"/>
+      <c r="B9" s="141"/>
       <c r="C9" s="3" t="s">
         <v>81</v>
       </c>
@@ -5440,19 +5417,19 @@
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="158"/>
-      <c r="B10" s="142"/>
+      <c r="B10" s="141"/>
       <c r="C10" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="158"/>
-      <c r="B11" s="142"/>
+      <c r="B11" s="141"/>
       <c r="C11" s="3" t="s">
         <v>83</v>
       </c>
@@ -5461,60 +5438,60 @@
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="158"/>
-      <c r="B12" s="142"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="10"/>
       <c r="F12" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="158"/>
-      <c r="B13" s="142"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="10"/>
       <c r="F13" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="158"/>
-      <c r="B14" s="142"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="10"/>
       <c r="F14" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="158"/>
-      <c r="B15" s="142"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="3" t="s">
         <v>95</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="10"/>
       <c r="F15" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="158"/>
-      <c r="B16" s="142"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="3" t="s">
         <v>176</v>
       </c>
@@ -5524,43 +5501,43 @@
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="158"/>
-      <c r="B17" s="142"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="3" t="s">
         <v>177</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="10"/>
       <c r="F17" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="158"/>
-      <c r="B18" s="142"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="3" t="s">
         <v>178</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="10"/>
       <c r="F18" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="158"/>
-      <c r="B19" s="142"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="3" t="s">
         <v>179</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="10"/>
       <c r="F19" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="158"/>
-      <c r="B20" s="142"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="3" t="s">
         <v>87</v>
       </c>
@@ -5569,12 +5546,12 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="158"/>
-      <c r="B21" s="142"/>
+      <c r="B21" s="141"/>
       <c r="C21" s="3" t="s">
         <v>87</v>
       </c>
@@ -5583,50 +5560,50 @@
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="158"/>
-      <c r="B22" s="142"/>
+      <c r="B22" s="141"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
         <v>182</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="158"/>
-      <c r="B23" s="142"/>
+      <c r="B23" s="141"/>
       <c r="C23" s="10"/>
       <c r="D23" s="3" t="s">
         <v>183</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="159"/>
-      <c r="B24" s="143"/>
+      <c r="B24" s="142"/>
       <c r="C24" s="8"/>
       <c r="D24" s="4" t="s">
         <v>184</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="157">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B25" s="141" t="s">
+      <c r="B25" s="140" t="s">
         <v>88</v>
       </c>
       <c r="C25" s="26"/>
@@ -5636,7 +5613,7 @@
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="158"/>
-      <c r="B26" s="142"/>
+      <c r="B26" s="141"/>
       <c r="C26" s="3" t="s">
         <v>89</v>
       </c>
@@ -5650,33 +5627,33 @@
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="158"/>
-      <c r="B27" s="142"/>
+      <c r="B27" s="141"/>
       <c r="C27" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="158"/>
-      <c r="B28" s="142"/>
+      <c r="B28" s="141"/>
       <c r="C28" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="158"/>
-      <c r="B29" s="142"/>
+      <c r="B29" s="141"/>
       <c r="C29" s="3" t="s">
         <v>84</v>
       </c>
@@ -5685,50 +5662,50 @@
         <v>17</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="158"/>
-      <c r="B30" s="142"/>
+      <c r="B30" s="141"/>
       <c r="C30" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="10"/>
       <c r="F30" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="158"/>
-      <c r="B31" s="142"/>
+      <c r="B31" s="141"/>
       <c r="C31" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="10"/>
       <c r="F31" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="159"/>
-      <c r="B32" s="143"/>
+      <c r="B32" s="142"/>
       <c r="C32" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="8"/>
       <c r="F32" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="157">
         <v>2.4</v>
       </c>
-      <c r="B33" s="141" t="s">
+      <c r="B33" s="140" t="s">
         <v>90</v>
       </c>
       <c r="C33" s="27"/>
@@ -5738,7 +5715,7 @@
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="158"/>
-      <c r="B34" s="142"/>
+      <c r="B34" s="141"/>
       <c r="C34" s="3" t="s">
         <v>91</v>
       </c>
@@ -5750,33 +5727,33 @@
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="158"/>
-      <c r="B35" s="142"/>
+      <c r="B35" s="141"/>
       <c r="C35" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="158"/>
-      <c r="B36" s="142"/>
+      <c r="B36" s="141"/>
       <c r="C36" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="158"/>
-      <c r="B37" s="142"/>
+      <c r="B37" s="141"/>
       <c r="C37" s="3" t="s">
         <v>84</v>
       </c>
@@ -5785,50 +5762,50 @@
         <v>17</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="158"/>
-      <c r="B38" s="142"/>
+      <c r="B38" s="141"/>
       <c r="C38" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="10"/>
       <c r="F38" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="158"/>
-      <c r="B39" s="142"/>
+      <c r="B39" s="141"/>
       <c r="C39" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="10"/>
       <c r="F39" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="159"/>
-      <c r="B40" s="143"/>
+      <c r="B40" s="142"/>
       <c r="C40" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="8"/>
       <c r="F40" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="157">
         <v>2.5</v>
       </c>
-      <c r="B41" s="141" t="s">
+      <c r="B41" s="140" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="27"/>
@@ -5838,7 +5815,7 @@
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="158"/>
-      <c r="B42" s="142"/>
+      <c r="B42" s="141"/>
       <c r="C42" s="22"/>
       <c r="D42" s="3" t="s">
         <v>93</v>
@@ -5850,19 +5827,19 @@
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="158"/>
-      <c r="B43" s="142"/>
+      <c r="B43" s="141"/>
       <c r="C43" s="22"/>
       <c r="D43" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="158"/>
-      <c r="B44" s="142"/>
+      <c r="B44" s="141"/>
       <c r="C44" s="22"/>
       <c r="D44" s="3" t="s">
         <v>83</v>
@@ -5871,76 +5848,76 @@
         <v>96</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="158"/>
-      <c r="B45" s="142"/>
+      <c r="B45" s="141"/>
       <c r="C45" s="22"/>
       <c r="D45" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="158"/>
-      <c r="B46" s="142"/>
+      <c r="B46" s="141"/>
       <c r="C46" s="22"/>
       <c r="D46" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="158"/>
-      <c r="B47" s="142"/>
+      <c r="B47" s="141"/>
       <c r="C47" s="22"/>
       <c r="D47" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="158"/>
-      <c r="B48" s="142"/>
+      <c r="B48" s="141"/>
       <c r="C48" s="22"/>
       <c r="D48" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="159"/>
-      <c r="B49" s="143"/>
+      <c r="B49" s="142"/>
       <c r="C49" s="14"/>
       <c r="D49" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="157">
         <v>2.6</v>
       </c>
-      <c r="B50" s="141" t="s">
+      <c r="B50" s="140" t="s">
         <v>97</v>
       </c>
       <c r="C50" s="21"/>
@@ -5950,7 +5927,7 @@
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="158"/>
-      <c r="B51" s="142"/>
+      <c r="B51" s="141"/>
       <c r="C51" s="22" t="s">
         <v>17</v>
       </c>
@@ -5964,83 +5941,83 @@
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="158"/>
-      <c r="B52" s="142"/>
+      <c r="B52" s="141"/>
       <c r="C52" s="22"/>
       <c r="D52" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="158"/>
-      <c r="B53" s="142"/>
+      <c r="B53" s="141"/>
       <c r="C53" s="22"/>
       <c r="D53" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="158"/>
-      <c r="B54" s="142"/>
+      <c r="B54" s="141"/>
       <c r="C54" s="22"/>
       <c r="D54" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="158"/>
-      <c r="B55" s="142"/>
+      <c r="B55" s="141"/>
       <c r="C55" s="22"/>
       <c r="D55" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="158"/>
-      <c r="B56" s="142"/>
+      <c r="B56" s="141"/>
       <c r="C56" s="22"/>
       <c r="D56" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="159"/>
-      <c r="B57" s="143"/>
+      <c r="B57" s="142"/>
       <c r="C57" s="14"/>
       <c r="D57" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="157">
         <v>2.7</v>
       </c>
-      <c r="B58" s="141" t="s">
+      <c r="B58" s="140" t="s">
         <v>99</v>
       </c>
       <c r="C58" s="21"/>
@@ -6050,7 +6027,7 @@
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="158"/>
-      <c r="B59" s="142"/>
+      <c r="B59" s="141"/>
       <c r="C59" s="22"/>
       <c r="D59" s="3" t="s">
         <v>100</v>
@@ -6062,81 +6039,81 @@
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="158"/>
-      <c r="B60" s="142"/>
+      <c r="B60" s="141"/>
       <c r="C60" s="22"/>
       <c r="D60" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E60" s="16"/>
       <c r="F60" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="158"/>
-      <c r="B61" s="142"/>
+      <c r="B61" s="141"/>
       <c r="C61" s="22"/>
       <c r="D61" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E61" s="16"/>
       <c r="F61" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="158"/>
-      <c r="B62" s="142"/>
+      <c r="B62" s="141"/>
       <c r="C62" s="22"/>
       <c r="D62" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E62" s="16"/>
       <c r="F62" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="158"/>
-      <c r="B63" s="142"/>
+      <c r="B63" s="141"/>
       <c r="C63" s="22"/>
       <c r="D63" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E63" s="16"/>
       <c r="F63" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="158"/>
-      <c r="B64" s="142"/>
+      <c r="B64" s="141"/>
       <c r="C64" s="22"/>
       <c r="D64" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E64" s="16"/>
       <c r="F64" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="159"/>
-      <c r="B65" s="143"/>
+      <c r="B65" s="142"/>
       <c r="C65" s="14"/>
       <c r="D65" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="141">
+      <c r="A66" s="140">
         <v>2.8</v>
       </c>
-      <c r="B66" s="141" t="s">
+      <c r="B66" s="140" t="s">
         <v>101</v>
       </c>
       <c r="C66" s="21"/>
@@ -6145,8 +6122,8 @@
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="142"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="141"/>
+      <c r="B67" s="141"/>
       <c r="C67" s="22"/>
       <c r="D67" s="3" t="s">
         <v>102</v>
@@ -6155,87 +6132,87 @@
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="142"/>
-      <c r="B68" s="142"/>
+      <c r="A68" s="141"/>
+      <c r="B68" s="141"/>
       <c r="C68" s="22"/>
       <c r="D68" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="142"/>
-      <c r="B69" s="142"/>
+      <c r="A69" s="141"/>
+      <c r="B69" s="141"/>
       <c r="C69" s="22"/>
       <c r="D69" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E69" s="16"/>
       <c r="F69" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="142"/>
-      <c r="B70" s="142"/>
+      <c r="A70" s="141"/>
+      <c r="B70" s="141"/>
       <c r="C70" s="22"/>
       <c r="D70" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E70" s="16"/>
       <c r="F70" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="142"/>
-      <c r="B71" s="142"/>
+      <c r="A71" s="141"/>
+      <c r="B71" s="141"/>
       <c r="C71" s="22"/>
       <c r="D71" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E71" s="16"/>
       <c r="F71" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="142"/>
-      <c r="B72" s="142"/>
+      <c r="A72" s="141"/>
+      <c r="B72" s="141"/>
       <c r="C72" s="22"/>
       <c r="D72" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E72" s="16"/>
       <c r="F72" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="142"/>
-      <c r="B73" s="142"/>
+      <c r="A73" s="141"/>
+      <c r="B73" s="141"/>
       <c r="C73" s="22"/>
       <c r="D73" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E73" s="16"/>
       <c r="F73" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="143"/>
-      <c r="B74" s="143"/>
+      <c r="A74" s="142"/>
+      <c r="B74" s="142"/>
       <c r="C74" s="14"/>
       <c r="D74" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -6398,13 +6375,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
-    <mergeCell ref="A8:A24"/>
-    <mergeCell ref="B8:B24"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A66:A74"/>
     <mergeCell ref="B66:B74"/>
@@ -6421,6 +6391,13 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A8:A24"/>
+    <mergeCell ref="B8:B24"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6435,7 +6412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BI231"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6450,30 +6429,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="104" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="140" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
+      <c r="A2" s="155" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
     </row>
     <row r="3" spans="1:6" s="104" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="E4" s="143" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -6481,20 +6460,20 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="172"/>
-      <c r="B5" s="173"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
+      <c r="A5" s="160"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
       <c r="F5" s="73" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="149">
+      <c r="A6" s="151">
         <v>3.1</v>
       </c>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>207</v>
       </c>
       <c r="C6" s="54"/>
@@ -6504,115 +6483,115 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="161"/>
-      <c r="B7" s="145"/>
+      <c r="B7" s="146"/>
       <c r="C7" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" s="70"/>
       <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="161"/>
-      <c r="B8" s="145"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="55" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E8" s="70"/>
       <c r="F8" s="74" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="161"/>
-      <c r="B9" s="145"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E9" s="70"/>
       <c r="F9" s="74" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="161"/>
-      <c r="B10" s="145"/>
+      <c r="B10" s="146"/>
       <c r="C10" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E10" s="71" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F10" s="74"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="161"/>
-      <c r="B11" s="145"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E11" s="70"/>
       <c r="F11" s="74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="161"/>
-      <c r="B12" s="145"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" s="70"/>
       <c r="F12" s="74" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="161"/>
-      <c r="B13" s="145"/>
+      <c r="B13" s="146"/>
       <c r="C13" s="55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" s="70"/>
       <c r="F13" s="74" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="161"/>
-      <c r="B14" s="145"/>
+      <c r="B14" s="146"/>
       <c r="C14" s="55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E14" s="70"/>
       <c r="F14" s="74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="161"/>
-      <c r="B15" s="145"/>
+      <c r="B15" s="146"/>
       <c r="C15" s="56" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E15" s="70"/>
       <c r="F15" s="75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="161"/>
-      <c r="B16" s="145"/>
+      <c r="B16" s="146"/>
       <c r="C16" s="57"/>
       <c r="D16" s="63"/>
       <c r="E16" s="70"/>
       <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="160">
+      <c r="A17" s="172">
         <v>3.2</v>
       </c>
-      <c r="B17" s="144" t="s">
-        <v>208</v>
+      <c r="B17" s="145" t="s">
+        <v>331</v>
       </c>
       <c r="C17" s="58"/>
       <c r="D17" s="64"/>
@@ -6621,31 +6600,31 @@
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="161"/>
-      <c r="B18" s="145"/>
+      <c r="B18" s="146"/>
       <c r="C18" s="59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="162"/>
-      <c r="B19" s="146"/>
+      <c r="A19" s="173"/>
+      <c r="B19" s="156"/>
       <c r="C19" s="60"/>
       <c r="D19" s="66"/>
       <c r="E19" s="60"/>
       <c r="F19" s="34"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="160">
+      <c r="A20" s="172">
         <v>3.3</v>
       </c>
-      <c r="B20" s="144" t="s">
+      <c r="B20" s="145" t="s">
         <v>104</v>
       </c>
       <c r="C20" s="59"/>
@@ -6657,7 +6636,7 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="161"/>
-      <c r="B21" s="145"/>
+      <c r="B21" s="146"/>
       <c r="C21" s="59" t="s">
         <v>105</v>
       </c>
@@ -6667,7 +6646,7 @@
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="161"/>
-      <c r="B22" s="145"/>
+      <c r="B22" s="146"/>
       <c r="C22" s="59" t="s">
         <v>185</v>
       </c>
@@ -6676,28 +6655,28 @@
       </c>
       <c r="E22" s="70"/>
       <c r="F22" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="162"/>
-      <c r="B23" s="146"/>
+      <c r="A23" s="173"/>
+      <c r="B23" s="156"/>
       <c r="C23" s="61" t="s">
         <v>186</v>
       </c>
       <c r="D23" s="67"/>
       <c r="E23" s="77" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F23" s="76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="160">
+      <c r="A24" s="172">
         <v>3.4</v>
       </c>
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="145" t="s">
         <v>107</v>
       </c>
       <c r="C24" s="165" t="s">
@@ -6705,25 +6684,25 @@
       </c>
       <c r="D24" s="170"/>
       <c r="E24" s="167" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F24" s="168" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="161"/>
-      <c r="B25" s="145"/>
+      <c r="B25" s="146"/>
       <c r="C25" s="166"/>
       <c r="D25" s="171"/>
       <c r="E25" s="167"/>
       <c r="F25" s="169"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="149">
+      <c r="A26" s="151">
         <v>3.5</v>
       </c>
-      <c r="B26" s="163" t="s">
+      <c r="B26" s="162" t="s">
         <v>109</v>
       </c>
       <c r="C26" s="58"/>
@@ -6733,7 +6712,7 @@
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="161"/>
-      <c r="B27" s="145"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="59"/>
       <c r="D27" s="63" t="s">
         <v>110</v>
@@ -6745,30 +6724,30 @@
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="161"/>
-      <c r="B28" s="145"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="59"/>
       <c r="D28" s="63" t="s">
         <v>187</v>
       </c>
       <c r="E28" s="70" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="150"/>
+      <c r="A29" s="152"/>
       <c r="B29" s="164"/>
       <c r="C29" s="62"/>
       <c r="D29" s="69" t="s">
         <v>111</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
@@ -6976,8 +6955,19 @@
     <row r="230" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="231" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A16"/>
@@ -6986,18 +6976,6 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -7028,30 +7006,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="104" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
+      <c r="A2" s="182" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
     </row>
     <row r="3" spans="1:6" s="104" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="E4" s="143" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -7059,20 +7037,20 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="154"/>
-      <c r="B5" s="156"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
+      <c r="A5" s="144"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
       <c r="F5" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="141">
+      <c r="A6" s="140">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="140" t="s">
         <v>113</v>
       </c>
       <c r="C6" s="17"/>
@@ -7083,36 +7061,36 @@
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="142"/>
-      <c r="B7" s="142"/>
+      <c r="A7" s="141"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="18"/>
       <c r="D7" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
-      <c r="B8" s="142"/>
+      <c r="A8" s="141"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="46"/>
       <c r="D8" s="36" t="s">
         <v>115</v>
       </c>
       <c r="E8" s="44"/>
       <c r="F8" s="45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="141">
+      <c r="A9" s="140">
         <v>4.2</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="140" t="s">
         <v>116</v>
       </c>
       <c r="C9" s="5"/>
@@ -7123,100 +7101,100 @@
       <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="142"/>
-      <c r="B10" s="142"/>
+      <c r="A10" s="141"/>
+      <c r="B10" s="141"/>
       <c r="C10" s="3" t="s">
         <v>117</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="142"/>
-      <c r="B11" s="142"/>
+      <c r="A11" s="141"/>
+      <c r="B11" s="141"/>
       <c r="C11" s="3"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="142"/>
-      <c r="B12" s="142"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="141"/>
       <c r="C12" s="3" t="s">
         <v>124</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="142"/>
-      <c r="B13" s="142"/>
+      <c r="A13" s="141"/>
+      <c r="B13" s="141"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="142"/>
-      <c r="B14" s="142"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="142"/>
-      <c r="B15" s="142"/>
+      <c r="A15" s="141"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="10"/>
       <c r="D15" s="3" t="s">
         <v>127</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="143"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="142"/>
       <c r="C16" s="8"/>
       <c r="D16" s="4" t="s">
         <v>128</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="141">
+      <c r="A17" s="140">
         <v>4.3</v>
       </c>
-      <c r="B17" s="141" t="s">
+      <c r="B17" s="140" t="s">
         <v>118</v>
       </c>
       <c r="C17" s="26"/>
@@ -7225,8 +7203,8 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="142"/>
-      <c r="B18" s="142"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="3" t="s">
         <v>119</v>
       </c>
@@ -7237,58 +7215,58 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="142"/>
-      <c r="B19" s="142"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="143"/>
+      <c r="A20" s="142"/>
+      <c r="B20" s="142"/>
       <c r="C20" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="141">
+      <c r="A21" s="140">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="140" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="179" t="s">
+      <c r="C21" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="181"/>
-      <c r="E21" s="175" t="s">
+      <c r="D21" s="180"/>
+      <c r="E21" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="177" t="s">
-        <v>317</v>
+      <c r="F21" s="176" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="182"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="178"/>
+      <c r="A22" s="142"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="181"/>
+      <c r="E22" s="175"/>
+      <c r="F22" s="177"/>
     </row>
     <row r="23" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="50"/>
@@ -7596,12 +7574,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
@@ -7614,6 +7586,12 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="4" orientation="portrait"/>

</xml_diff>